<commit_message>
update age ratios and heatmaps
</commit_message>
<xml_diff>
--- a/data_input/00_data_sources.xlsx
+++ b/data_input/00_data_sources.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>https://www150.statcan.gc.ca/t1/tbl1/en/tv.action?pid=1710005701</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>DecesSemaine_QC_GrAge.xlsx</t>
+  </si>
+  <si>
+    <t>https://covid-19.ontario.ca/</t>
   </si>
 </sst>
 </file>
@@ -481,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -562,6 +565,9 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -621,8 +627,9 @@
     <hyperlink ref="D14" r:id="rId8" location="data-export"/>
     <hyperlink ref="C17" r:id="rId9" location="tri_pop=10"/>
     <hyperlink ref="C16" r:id="rId10"/>
+    <hyperlink ref="C9" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>